<commit_message>
Implemented Read Input Settings File - ForgetfulShrug 4/4/24
</commit_message>
<xml_diff>
--- a/RandomGameSelector/Resources/Test_Game_Lists.xlsx
+++ b/RandomGameSelector/Resources/Test_Game_Lists.xlsx
@@ -39,22 +39,22 @@
     <t>3DS 2</t>
   </si>
   <si>
-    <t>3DS 3</t>
+    <t>3DS Digi 3</t>
   </si>
   <si>
     <t>Digital</t>
   </si>
   <si>
-    <t>3DS 4</t>
-  </si>
-  <si>
-    <t>3DS 5</t>
-  </si>
-  <si>
-    <t>3DS 6</t>
-  </si>
-  <si>
-    <t>3DS 7</t>
+    <t>3DS Digi 4</t>
+  </si>
+  <si>
+    <t>3DS Digi 5</t>
+  </si>
+  <si>
+    <t>3DS Digi 6</t>
+  </si>
+  <si>
+    <t>3DS Digi 7</t>
   </si>
   <si>
     <t>3DS 8</t>
@@ -87,16 +87,16 @@
     <t>GBA 6</t>
   </si>
   <si>
-    <t>Switch 1</t>
+    <t>Switch Digi 1</t>
   </si>
   <si>
     <t>Switch</t>
   </si>
   <si>
-    <t>Switch 2</t>
-  </si>
-  <si>
-    <t>Switch 3</t>
+    <t>Switch Digi 2</t>
+  </si>
+  <si>
+    <t>Switch Digi 3</t>
   </si>
   <si>
     <t>Switch 4</t>
@@ -123,16 +123,16 @@
     <t>Wii U 4</t>
   </si>
   <si>
-    <t>Wii U 5</t>
-  </si>
-  <si>
-    <t>Wii U 6</t>
-  </si>
-  <si>
-    <t>Wii U 7</t>
-  </si>
-  <si>
-    <t>Wii U 8</t>
+    <t>Wii U Digi 5</t>
+  </si>
+  <si>
+    <t>Wii U Digi 6</t>
+  </si>
+  <si>
+    <t>Wii U Digi 7</t>
+  </si>
+  <si>
+    <t>Wii U Digi 8</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Various Forms Changes - Forgetful Shrug 4/7/24
</commit_message>
<xml_diff>
--- a/RandomGameSelector/Resources/Test_Game_Lists.xlsx
+++ b/RandomGameSelector/Resources/Test_Game_Lists.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Games_List" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Games_List!$A$1:$D$29</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Games_List!$A$1:$D$33</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="44">
   <si>
     <t>##Name</t>
   </si>
@@ -30,7 +30,7 @@
     <t>3DS 1</t>
   </si>
   <si>
-    <t>3DS</t>
+    <t>Nintendo 3DS</t>
   </si>
   <si>
     <t>Physical</t>
@@ -66,7 +66,7 @@
     <t>GBA 1</t>
   </si>
   <si>
-    <t>GBA</t>
+    <t>Nintendo GBA</t>
   </si>
   <si>
     <t>yes</t>
@@ -90,7 +90,7 @@
     <t>Switch Digi 1</t>
   </si>
   <si>
-    <t>Switch</t>
+    <t>Nintendo Switch</t>
   </si>
   <si>
     <t>Switch Digi 2</t>
@@ -108,10 +108,22 @@
     <t>Switch 5</t>
   </si>
   <si>
+    <t>Switch 6</t>
+  </si>
+  <si>
+    <t>Switch 7</t>
+  </si>
+  <si>
+    <t>Switch 8</t>
+  </si>
+  <si>
+    <t>Switch 9</t>
+  </si>
+  <si>
     <t>Wii U 1</t>
   </si>
   <si>
-    <t>Wii U</t>
+    <t>Nintendo Wii U</t>
   </si>
   <si>
     <t>Wii U 2</t>
@@ -745,8 +757,8 @@
       <c r="A22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>32</v>
+      <c r="B22" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>29</v>
@@ -757,10 +769,10 @@
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="12" t="s">
         <v>32</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>29</v>
@@ -771,10 +783,10 @@
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>29</v>
@@ -785,13 +797,13 @@
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>6</v>
+        <v>34</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>18</v>
@@ -799,13 +811,13 @@
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>9</v>
+      <c r="C26" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>18</v>
@@ -816,10 +828,10 @@
         <v>37</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>18</v>
@@ -830,30 +842,86 @@
         <v>38</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$D$29">
-    <sortState ref="A1:D29">
-      <sortCondition ref="B1:B29"/>
-      <sortCondition ref="A1:A29"/>
+  <autoFilter ref="$A$1:$D$33">
+    <sortState ref="A1:D33">
+      <sortCondition ref="B1:B33"/>
+      <sortCondition ref="A1:A33"/>
     </sortState>
   </autoFilter>
   <drawing r:id="rId1"/>

</xml_diff>